<commit_message>
Latest changes made to Add Teacher record vis Excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/TeacherDetails.xlsx
+++ b/src/test/resources/TeacherDetails.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6075"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Code</t>
   </si>
@@ -33,6 +33,45 @@
   </si>
   <si>
     <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Birth Date</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Marital Status</t>
+  </si>
+  <si>
+    <t>C001</t>
+  </si>
+  <si>
+    <t>Faisal</t>
+  </si>
+  <si>
+    <t>Javed</t>
+  </si>
+  <si>
+    <t>Khatri</t>
+  </si>
+  <si>
+    <t>13/05/1986</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Contact No</t>
+  </si>
+  <si>
+    <t>9324705330</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -68,8 +107,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,31 +393,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>